<commit_message>
chore: update the .gitignore file
</commit_message>
<xml_diff>
--- a/data/validation_set.xlsx
+++ b/data/validation_set.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rockmtnins-my.sharepoint.com/personal/hamidreza_zoraghein_rmi_org/Documents/Development/llm/rag_cft/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rockmtnins-my.sharepoint.com/personal/hamidreza_zoraghein_rmi_org/Documents/Development/rag_cft/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="57" documentId="8_{2D27B883-FC49-C14C-BAB8-CB60E64C3CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA13DE2E-2B5D-0D41-AE41-A3157A7C7D74}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3680" yWindow="4300" windowWidth="28040" windowHeight="15800" xr2:uid="{E8F754B0-06CB-C746-BCF9-8BE2A757031D}"/>
+    <workbookView xWindow="3680" yWindow="4300" windowWidth="28040" windowHeight="15800" xr2:uid="{E8F754B0-06CB-C746-BCF9-8BE2A757031D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -568,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC86DDE-7DA1-7642-8C1A-A7315B6109FD}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>